<commit_message>
new sat server setup
</commit_message>
<xml_diff>
--- a/dev/vmdefs.xlsx
+++ b/dev/vmdefs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01015B4F-2D4A-4DC4-95B9-33A663F53FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19795F68-F6EB-4237-A4E8-D4EBC45AF515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15285" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="vms" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="314">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1002,22 +1002,25 @@
     <t>FOLDER (ONLY FOR ESX)</t>
   </si>
   <si>
-    <t>LU718</t>
-  </si>
-  <si>
-    <t>VM TEST - LNX - MK417</t>
-  </si>
-  <si>
-    <t>lu718</t>
-  </si>
-  <si>
     <t>MEM(MB)</t>
   </si>
   <si>
-    <t>200.1.1.105</t>
-  </si>
-  <si>
-    <t>200.1.1.240</t>
+    <t>VSL-PRO-SAT-01</t>
+  </si>
+  <si>
+    <t>NEW SATELLITE SERVER 6.12</t>
+  </si>
+  <si>
+    <t>vsl-pro-sat-01</t>
+  </si>
+  <si>
+    <t>/DMZ/MGMT</t>
+  </si>
+  <si>
+    <t>172.22.56.11</t>
+  </si>
+  <si>
+    <t>172.22.56.1</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1408,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1476,7 @@
         <v>306</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
@@ -1499,63 +1502,67 @@
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>"sub_"&amp;G2</f>
-        <v>sub_cluster650</v>
+        <v>sub_nut-dmz-01</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="K2" s="3" t="str">
         <f>"stg_"&amp;G2</f>
-        <v>stg_cluster650</v>
+        <v>stg_nut-dmz-01</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>270</v>
+        <v>63</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="N2" s="2">
-        <v>2048</v>
+        <f>48*1024</f>
+        <v>49152</v>
       </c>
       <c r="O2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P2" s="2">
         <v>1</v>
       </c>
       <c r="Q2" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="S2" s="2">
         <v>24</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
adding lu717 and SAP DEV
</commit_message>
<xml_diff>
--- a/dev/vmdefs.xlsx
+++ b/dev/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB8A40D-EC64-4219-9FE7-3B7C61B98648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4642C4A3-FED2-4CDF-B1BC-BE719A6033FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15285" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="318">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1002,22 +1002,37 @@
     <t>FOLDER (ONLY FOR ESX)</t>
   </si>
   <si>
-    <t>LU718</t>
-  </si>
-  <si>
-    <t>lu718</t>
-  </si>
-  <si>
     <t>MEM(MB)</t>
   </si>
   <si>
-    <t>200.1.1.105</t>
-  </si>
-  <si>
     <t>200.1.1.240</t>
   </si>
   <si>
     <t>VM DE TEST - LNX</t>
+  </si>
+  <si>
+    <t>VSL-TST-SAP-001</t>
+  </si>
+  <si>
+    <t>APP Server SAP - TST</t>
+  </si>
+  <si>
+    <t>172.26.16.1</t>
+  </si>
+  <si>
+    <t>172.26.16.254</t>
+  </si>
+  <si>
+    <t>/DMZ/DEV</t>
+  </si>
+  <si>
+    <t>LU717</t>
+  </si>
+  <si>
+    <t>lu717</t>
+  </si>
+  <si>
+    <t>200.1.1.106</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1420,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1433,7 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="49.140625" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="46.5703125" bestFit="1" customWidth="1"/>
@@ -1473,7 +1488,7 @@
         <v>306</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
@@ -1502,16 +1517,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
@@ -1549,28 +1564,83 @@
         <v>100</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="S2" s="2">
         <v>24</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>sub_nut-dmz-02</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
+        <v>stg_nut-dmz-02</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="N3" s="2">
+        <v>16384</v>
+      </c>
+      <c r="O3" s="2">
+        <v>4</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>100</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="S3" s="2">
+        <v>24</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2529,7 +2599,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L54:M54" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M35:M53 L2:L53 G2:H53" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M35:M53 G2:H53 L2:L53" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F53" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
@@ -2548,13 +2618,13 @@
           <x14:formula1>
             <xm:f>params!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A52</xm:sqref>
+          <xm:sqref>A2 A4:A52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0B35C17-C684-46B2-AA38-9FA5534C30BF}">
           <x14:formula1>
             <xm:f>params!$C$3:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U53</xm:sqref>
+          <xm:sqref>U2 U4:U53</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
adding SAP QAL and PROD
</commit_message>
<xml_diff>
--- a/dev/vmdefs.xlsx
+++ b/dev/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4642C4A3-FED2-4CDF-B1BC-BE719A6033FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2F0F6D-E1EA-46DD-A098-83CCB4E4A02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15285" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="321">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1005,12 +1005,6 @@
     <t>MEM(MB)</t>
   </si>
   <si>
-    <t>200.1.1.240</t>
-  </si>
-  <si>
-    <t>VM DE TEST - LNX</t>
-  </si>
-  <si>
     <t>VSL-TST-SAP-001</t>
   </si>
   <si>
@@ -1026,13 +1020,28 @@
     <t>/DMZ/DEV</t>
   </si>
   <si>
-    <t>LU717</t>
-  </si>
-  <si>
-    <t>lu717</t>
-  </si>
-  <si>
-    <t>200.1.1.106</t>
+    <t>VSL-REC-SAP-001</t>
+  </si>
+  <si>
+    <t>APP Server SAP - QAL</t>
+  </si>
+  <si>
+    <t>172.25.16.1</t>
+  </si>
+  <si>
+    <t>172.25.16.254</t>
+  </si>
+  <si>
+    <t>VSL-PRO-SAP-001</t>
+  </si>
+  <si>
+    <t>APP Server SAP - PRO</t>
+  </si>
+  <si>
+    <t>172.23.16.1</t>
+  </si>
+  <si>
+    <t>172.23.16.254</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1427,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAEDD9-6941-4909-B148-BE39F1BC44CD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U54"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,48 +1523,51 @@
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>309</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="shared" ref="I2:I4" si="0">"sub_"&amp;G2</f>
-        <v>sub_cluster650</v>
+        <v>sub_nut-dmz-02</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K2" s="3" t="str">
         <f t="shared" ref="K2:K4" si="1">"stg_"&amp;G2</f>
-        <v>stg_cluster650</v>
+        <v>stg_nut-dmz-02</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>270</v>
+        <v>64</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="N2" s="2">
-        <v>2048</v>
+        <v>16384</v>
       </c>
       <c r="O2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P2" s="2">
         <v>1</v>
@@ -1564,13 +1576,13 @@
         <v>100</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="S2" s="2">
         <v>24</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>19</v>
@@ -1581,16 +1593,16 @@
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>37</v>
@@ -1606,7 +1618,7 @@
         <v>sub_nut-dmz-02</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1616,7 +1628,7 @@
         <v>64</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="N3" s="2">
         <v>16384</v>
@@ -1631,28 +1643,83 @@
         <v>100</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="S3" s="2">
         <v>24</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="3"/>
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>sub_nut-dmz-01</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="K4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
+        <v>stg_nut-dmz-01</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="N4" s="2">
+        <v>16384</v>
+      </c>
+      <c r="O4" s="2">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>100</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="S4" s="2">
+        <v>24</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -1661,12 +1728,12 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="str">
-        <f t="shared" ref="I5:I36" si="2">"sub_"&amp;G5</f>
+        <f t="shared" ref="I4:I35" si="2">"sub_"&amp;G5</f>
         <v>sub_</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="str">
-        <f t="shared" ref="K5:K53" si="3">"stg_"&amp;G5</f>
+        <f t="shared" ref="K4:K52" si="3">"stg_"&amp;G5</f>
         <v>stg_</v>
       </c>
       <c r="L5" s="2"/>
@@ -2250,7 +2317,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I36:I52" si="4">"sub_"&amp;G36</f>
         <v>sub_</v>
       </c>
       <c r="J36" s="3"/>
@@ -2269,7 +2336,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="str">
-        <f t="shared" ref="I37:I53" si="4">"sub_"&amp;G37</f>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J37" s="3"/>
@@ -2549,7 +2616,6 @@
       <c r="U51" s="2"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2568,44 +2634,26 @@
       <c r="U52" s="2"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
       <c r="H53" s="2"/>
-      <c r="I53" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>sub_</v>
-      </c>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>stg_</v>
-      </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="U53" s="2"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H54" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
-      <formula1>INDIRECT(G54)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H53" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
+      <formula1>INDIRECT(G53)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L54:M54" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L53:M53" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M35:M53 G2:H53 L2:L53" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M34:M52 G2:H52 L2:L52" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F53" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F52" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J53" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J52" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
       <formula1>INDIRECT(SUBSTITUTE(I2,"-","_"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2618,13 +2666,13 @@
           <x14:formula1>
             <xm:f>params!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2 A4:A52</xm:sqref>
+          <xm:sqref>A5:A51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0B35C17-C684-46B2-AA38-9FA5534C30BF}">
           <x14:formula1>
             <xm:f>params!$C$3:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>U2 U4:U53</xm:sqref>
+          <xm:sqref>U5:U52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
a new routine test
</commit_message>
<xml_diff>
--- a/dev/vmdefs.xlsx
+++ b/dev/vmdefs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FBA989-46B4-4ADF-9372-1B9C079BD2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B85015-7173-4EBA-9CAB-464EAAFE664E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15285" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="vms" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="318">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1018,6 +1018,21 @@
   </si>
   <si>
     <t>VM TEST LNX</t>
+  </si>
+  <si>
+    <t>VSL-POC-AIA-001</t>
+  </si>
+  <si>
+    <t>AIA POC LNX</t>
+  </si>
+  <si>
+    <t>vsl-poc-aia-001</t>
+  </si>
+  <si>
+    <t>192.168.25.106</t>
+  </si>
+  <si>
+    <t>192.168.25.1</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1421,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,23 +1579,69 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>sub_cluster651</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L3" s="2"/>
+        <v>stg_cluster651</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>296</v>
+      </c>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="N3" s="2">
+        <v>16384</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>100</v>
+      </c>
+      <c r="R3" t="s">
+        <v>316</v>
+      </c>
+      <c r="S3">
+        <v>24</v>
+      </c>
+      <c r="T3" t="s">
+        <v>317</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>